<commit_message>
calibrate probe sets for 2024 fieldwork
</commit_message>
<xml_diff>
--- a/arduino_settings/probe_calibrations.xlsx
+++ b/arduino_settings/probe_calibrations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcunning/Projects/pulchritude/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rcunning/Projects/pulchritude/arduino_settings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAB286B-0B46-F34B-B538-A787C44E630F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57299DD3-40E7-1A4F-9C42-3D481B6C4B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{5404584E-A39F-9042-8A99-28B15DF4B545}"/>
+    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="16940" xr2:uid="{5404584E-A39F-9042-8A99-28B15DF4B545}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="13">
   <si>
     <t>Box1probes</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>Box4probes</t>
+  </si>
+  <si>
+    <t>2024 experiments</t>
+  </si>
+  <si>
+    <t>Box5probes</t>
+  </si>
+  <si>
+    <t>Shedd_coral_traceable</t>
   </si>
 </sst>
 </file>
@@ -119,9 +128,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -159,7 +168,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -265,7 +274,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -407,7 +416,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -415,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD373BAD-953B-3043-8B2D-6244C0B20903}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -649,6 +658,159 @@
         <v>-0.41000000000000014</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>22.9</v>
+      </c>
+      <c r="C28">
+        <v>23.04</v>
+      </c>
+      <c r="D28">
+        <f>B28-C28</f>
+        <v>-0.14000000000000057</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>22.8</v>
+      </c>
+      <c r="C29">
+        <v>23.04</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ref="D29:D31" si="2">B29-C29</f>
+        <v>-0.23999999999999844</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>22.6</v>
+      </c>
+      <c r="C30">
+        <v>23.04</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>-0.43999999999999773</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>22.8</v>
+      </c>
+      <c r="C31">
+        <v>23.04</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>-0.23999999999999844</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34">
+        <v>22.1</v>
+      </c>
+      <c r="C34">
+        <v>22.47</v>
+      </c>
+      <c r="D34">
+        <f>B34-C34</f>
+        <v>-0.36999999999999744</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>21.8</v>
+      </c>
+      <c r="C35">
+        <v>22.47</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ref="D35:D37" si="3">B35-C35</f>
+        <v>-0.66999999999999815</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36">
+        <v>22.2</v>
+      </c>
+      <c r="C36">
+        <v>22.47</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="3"/>
+        <v>-0.26999999999999957</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>22.1</v>
+      </c>
+      <c r="C37">
+        <v>22.47</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="3"/>
+        <v>-0.36999999999999744</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>